<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-22.xlsx - 2026-01-22T10:16:31.142Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-22.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-22.xlsx
@@ -954,7 +954,7 @@
         <v>75</v>
       </c>
       <c r="H13" t="str">
-        <v>NEW</v>
+        <v>DELIVERED</v>
       </c>
       <c r="I13" t="str">
         <v>PENDING</v>
@@ -1198,7 +1198,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-22.xlsx - 2026-01-22T10:17:11.135Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-22.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-22.xlsx
@@ -517,7 +517,7 @@
         <v>DELIVERED</v>
       </c>
       <c r="I3" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J3" t="str">
         <v>2026-01-21</v>
@@ -1161,10 +1161,10 @@
         <v>170</v>
       </c>
       <c r="F2">
-        <v>60</v>
+        <v>170</v>
       </c>
       <c r="G2">
-        <v>110</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>